<commit_message>
feat: Advanced quiz system with randomization & question pooling
✨ Features:
- 📊 Import quiz from Excel with 30 sample questions (JS/React/HTML/CSS)
- 🔀 Shuffle questions (randomize): แต่ละคนได้ลำดับคำถามต่างกัน
- 🎲 Shuffle options: สุ่มลำดับตัวเลือก A,B,C,D แต่ละคนได้ลำดับต่างกัน
- 🎯 Question pooling: นำเข้า 30 ข้อ แต่ให้ทำ 20 ข้อ (สุ่มเลือกจากคลัง)
- ⏱️ Time limit: กำหนดเวลาทำข้อสอบได้ (นาที)
- 📝 Improved Excel template: ตัวอย่างข้อสอบคุณภาพสูง

🔧 Technical:
- Updated Quiz schema (shuffleOptions, questionPoolSize, questionsToShow)
- New getQuizForStudent() action with Fisher-Yates shuffle
- Enhanced ExcelImportForm UI with Thai labels & examples
- Auto-generate quiz-template.xlsx with 30 questions

🎨 UX Improvements:
- Clear labels & tooltips in Thai
- Visual example info card
- Better error messages
- Responsive form layout
</commit_message>
<xml_diff>
--- a/public/quiz-template.xlsx
+++ b/public/quiz-template.xlsx
@@ -397,10 +397,18 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1:F4"/>
+  <dimension ref="A1:F31"/>
   <sheetViews>
     <sheetView workbookViewId="0"/>
   </sheetViews>
+  <cols>
+    <col min="1" max="1" width="60.83203125" customWidth="1"/>
+    <col min="2" max="2" width="40.83203125" customWidth="1"/>
+    <col min="3" max="3" width="40.83203125" customWidth="1"/>
+    <col min="4" max="4" width="40.83203125" customWidth="1"/>
+    <col min="5" max="5" width="40.83203125" customWidth="1"/>
+    <col min="6" max="6" width="15.83203125" customWidth="1"/>
+  </cols>
   <sheetData>
     <row r="1">
       <c r="A1" t="str">
@@ -424,67 +432,607 @@
     </row>
     <row r="2">
       <c r="A2" t="str">
-        <v>What is the capital city of France?</v>
+        <v>JavaScript ย่อมาจากอะไร?</v>
       </c>
       <c r="B2" t="str">
-        <v>London</v>
+        <v>Just Another Very Awesome Script</v>
       </c>
       <c r="C2" t="str">
-        <v>Berlin</v>
+        <v>A scripting language for web development</v>
       </c>
       <c r="D2" t="str">
-        <v>Paris</v>
+        <v>Java Standard</v>
       </c>
       <c r="E2" t="str">
-        <v>Madrid</v>
+        <v>None of the above</v>
       </c>
       <c r="F2" t="str">
-        <v>C</v>
+        <v>B</v>
       </c>
     </row>
     <row r="3">
       <c r="A3" t="str">
-        <v>Which programming language is commonly used for web development?</v>
+        <v>ข้อใดคือ Data Type ใน JavaScript?</v>
       </c>
       <c r="B3" t="str">
-        <v>Python</v>
+        <v>String</v>
       </c>
       <c r="C3" t="str">
-        <v>JavaScript</v>
+        <v>Number</v>
       </c>
       <c r="D3" t="str">
-        <v>C++</v>
+        <v>Boolean</v>
       </c>
       <c r="E3" t="str">
-        <v>Java</v>
+        <v>ถูกทุกข้อ</v>
       </c>
       <c r="F3" t="str">
-        <v>B</v>
+        <v>D</v>
       </c>
     </row>
     <row r="4">
       <c r="A4" t="str">
-        <v>What does HTML stand for?</v>
+        <v>คำสั่งใดใช้แสดงผลใน Console?</v>
       </c>
       <c r="B4" t="str">
-        <v>Hyperlink Text Markup Language</v>
+        <v>console.log()</v>
       </c>
       <c r="C4" t="str">
+        <v>print()</v>
+      </c>
+      <c r="D4" t="str">
+        <v>echo()</v>
+      </c>
+      <c r="E4" t="str">
+        <v>display()</v>
+      </c>
+      <c r="F4" t="str">
+        <v>A</v>
+      </c>
+    </row>
+    <row r="5">
+      <c r="A5" t="str">
+        <v>ตัวแปรใน JavaScript ประกาศด้วยคำสั่งใด?</v>
+      </c>
+      <c r="B5" t="str">
+        <v>var, let, const</v>
+      </c>
+      <c r="C5" t="str">
+        <v>int, float, string</v>
+      </c>
+      <c r="D5" t="str">
+        <v>variable, data, value</v>
+      </c>
+      <c r="E5" t="str">
+        <v>declare, define, set</v>
+      </c>
+      <c r="F5" t="str">
+        <v>A</v>
+      </c>
+    </row>
+    <row r="6">
+      <c r="A6" t="str">
+        <v>Array ใน JavaScript เริ่มต้นที่ index เท่าไหร่?</v>
+      </c>
+      <c r="B6" t="str">
+        <v>1</v>
+      </c>
+      <c r="C6" t="str">
+        <v>0</v>
+      </c>
+      <c r="D6" t="str">
+        <v>-1</v>
+      </c>
+      <c r="E6" t="str">
+        <v>ขึ้นอยู่กับตัวแปร</v>
+      </c>
+      <c r="F6" t="str">
+        <v>B</v>
+      </c>
+    </row>
+    <row r="7">
+      <c r="A7" t="str">
+        <v>Function ใน JavaScript ประกาศอย่างไร?</v>
+      </c>
+      <c r="B7" t="str">
+        <v>function myFunc() {}</v>
+      </c>
+      <c r="C7" t="str">
+        <v>def myFunc() {}</v>
+      </c>
+      <c r="D7" t="str">
+        <v>void myFunc() {}</v>
+      </c>
+      <c r="E7" t="str">
+        <v>func myFunc() {}</v>
+      </c>
+      <c r="F7" t="str">
+        <v>A</v>
+      </c>
+    </row>
+    <row r="8">
+      <c r="A8" t="str">
+        <v>ข้อใดคือ Loop ใน JavaScript?</v>
+      </c>
+      <c r="B8" t="str">
+        <v>for</v>
+      </c>
+      <c r="C8" t="str">
+        <v>while</v>
+      </c>
+      <c r="D8" t="str">
+        <v>do-while</v>
+      </c>
+      <c r="E8" t="str">
+        <v>ถูกทุกข้อ</v>
+      </c>
+      <c r="F8" t="str">
+        <v>D</v>
+      </c>
+    </row>
+    <row r="9">
+      <c r="A9" t="str">
+        <v>Object ใน JavaScript สร้างด้วยเครื่องหมายอะไร?</v>
+      </c>
+      <c r="B9" t="str">
+        <v>[]</v>
+      </c>
+      <c r="C9" t="str">
+        <v>{}</v>
+      </c>
+      <c r="D9" t="str">
+        <v>()</v>
+      </c>
+      <c r="E9" t="str">
+        <v>&lt;&gt;</v>
+      </c>
+      <c r="F9" t="str">
+        <v>B</v>
+      </c>
+    </row>
+    <row r="10">
+      <c r="A10" t="str">
+        <v>Promise ใน JavaScript ใช้ทำอะไร?</v>
+      </c>
+      <c r="B10" t="str">
+        <v>Asynchronous programming</v>
+      </c>
+      <c r="C10" t="str">
+        <v>Create variables</v>
+      </c>
+      <c r="D10" t="str">
+        <v>Define functions</v>
+      </c>
+      <c r="E10" t="str">
+        <v>Loop through arrays</v>
+      </c>
+      <c r="F10" t="str">
+        <v>A</v>
+      </c>
+    </row>
+    <row r="11">
+      <c r="A11" t="str">
+        <v>Event Listener ใช้คำสั่งใด?</v>
+      </c>
+      <c r="B11" t="str">
+        <v>addEventListener()</v>
+      </c>
+      <c r="C11" t="str">
+        <v>addEvent()</v>
+      </c>
+      <c r="D11" t="str">
+        <v>listen()</v>
+      </c>
+      <c r="E11" t="str">
+        <v>on()</v>
+      </c>
+      <c r="F11" t="str">
+        <v>A</v>
+      </c>
+    </row>
+    <row r="12">
+      <c r="A12" t="str">
+        <v>HTML ย่อมาจากอะไร?</v>
+      </c>
+      <c r="B12" t="str">
+        <v>Hypertext Markup Language</v>
+      </c>
+      <c r="C12" t="str">
+        <v>High Text Markup Language</v>
+      </c>
+      <c r="D12" t="str">
+        <v>Hyper Transfer Markup Language</v>
+      </c>
+      <c r="E12" t="str">
         <v>Home Tool Markup Language</v>
       </c>
-      <c r="D4" t="str">
-        <v>HyperText Markup Language</v>
-      </c>
-      <c r="E4" t="str">
-        <v>Hyperlink and Text Markup Language</v>
-      </c>
-      <c r="F4" t="str">
-        <v>C</v>
+      <c r="F12" t="str">
+        <v>A</v>
+      </c>
+    </row>
+    <row r="13">
+      <c r="A13" t="str">
+        <v>CSS ใช้ทำอะไร?</v>
+      </c>
+      <c r="B13" t="str">
+        <v>จัดรูปแบบหน้าเว็บ</v>
+      </c>
+      <c r="C13" t="str">
+        <v>เขียนโปรแกรม</v>
+      </c>
+      <c r="D13" t="str">
+        <v>จัดการฐานข้อมูล</v>
+      </c>
+      <c r="E13" t="str">
+        <v>สร้าง API</v>
+      </c>
+      <c r="F13" t="str">
+        <v>A</v>
+      </c>
+    </row>
+    <row r="14">
+      <c r="A14" t="str">
+        <v>Tag ใดใช้สร้างลิงก์?</v>
+      </c>
+      <c r="B14" t="str">
+        <v>&lt;a&gt;</v>
+      </c>
+      <c r="C14" t="str">
+        <v>&lt;link&gt;</v>
+      </c>
+      <c r="D14" t="str">
+        <v>&lt;url&gt;</v>
+      </c>
+      <c r="E14" t="str">
+        <v>&lt;href&gt;</v>
+      </c>
+      <c r="F14" t="str">
+        <v>A</v>
+      </c>
+    </row>
+    <row r="15">
+      <c r="A15" t="str">
+        <v>Tag ใดใช้แสดงรูปภาพ?</v>
+      </c>
+      <c r="B15" t="str">
+        <v>&lt;img&gt;</v>
+      </c>
+      <c r="C15" t="str">
+        <v>&lt;image&gt;</v>
+      </c>
+      <c r="D15" t="str">
+        <v>&lt;picture&gt;</v>
+      </c>
+      <c r="E15" t="str">
+        <v>&lt;photo&gt;</v>
+      </c>
+      <c r="F15" t="str">
+        <v>A</v>
+      </c>
+    </row>
+    <row r="16">
+      <c r="A16" t="str">
+        <v>Responsive Design ใช้ Media Query อย่างไร?</v>
+      </c>
+      <c r="B16" t="str">
+        <v>@media screen and (max-width: 768px)</v>
+      </c>
+      <c r="C16" t="str">
+        <v>@responsive (max-width: 768px)</v>
+      </c>
+      <c r="D16" t="str">
+        <v>@screen (max-width: 768px)</v>
+      </c>
+      <c r="E16" t="str">
+        <v>@device (max-width: 768px)</v>
+      </c>
+      <c r="F16" t="str">
+        <v>A</v>
+      </c>
+    </row>
+    <row r="17">
+      <c r="A17" t="str">
+        <v>Flexbox ใช้ display เป็นอะไร?</v>
+      </c>
+      <c r="B17" t="str">
+        <v>flex</v>
+      </c>
+      <c r="C17" t="str">
+        <v>flexbox</v>
+      </c>
+      <c r="D17" t="str">
+        <v>flexible</v>
+      </c>
+      <c r="E17" t="str">
+        <v>flex-box</v>
+      </c>
+      <c r="F17" t="str">
+        <v>A</v>
+      </c>
+    </row>
+    <row r="18">
+      <c r="A18" t="str">
+        <v>Grid Layout ใช้ property ใดกำหนดคอลัมน์?</v>
+      </c>
+      <c r="B18" t="str">
+        <v>grid-template-columns</v>
+      </c>
+      <c r="C18" t="str">
+        <v>columns</v>
+      </c>
+      <c r="D18" t="str">
+        <v>grid-columns</v>
+      </c>
+      <c r="E18" t="str">
+        <v>template-columns</v>
+      </c>
+      <c r="F18" t="str">
+        <v>A</v>
+      </c>
+    </row>
+    <row r="19">
+      <c r="A19" t="str">
+        <v>Position: absolute จะอ้างอิงกับอะไร?</v>
+      </c>
+      <c r="B19" t="str">
+        <v>Parent ที่มี position: relative</v>
+      </c>
+      <c r="C19" t="str">
+        <v>Window</v>
+      </c>
+      <c r="D19" t="str">
+        <v>Body</v>
+      </c>
+      <c r="E19" t="str">
+        <v>Document</v>
+      </c>
+      <c r="F19" t="str">
+        <v>A</v>
+      </c>
+    </row>
+    <row r="20">
+      <c r="A20" t="str">
+        <v>z-index ใช้ทำอะไร?</v>
+      </c>
+      <c r="B20" t="str">
+        <v>กำหนดลำดับชั้น</v>
+      </c>
+      <c r="C20" t="str">
+        <v>กำหนดความกว้าง</v>
+      </c>
+      <c r="D20" t="str">
+        <v>กำหนดความสูง</v>
+      </c>
+      <c r="E20" t="str">
+        <v>กำหนดสี</v>
+      </c>
+      <c r="F20" t="str">
+        <v>A</v>
+      </c>
+    </row>
+    <row r="21">
+      <c r="A21" t="str">
+        <v>Pseudo-class :hover ใช้ทำอะไร?</v>
+      </c>
+      <c r="B21" t="str">
+        <v>เปลี่ยนสไตล์เมื่อชี้เมาส์</v>
+      </c>
+      <c r="C21" t="str">
+        <v>เปลี่ยนสีพื้นหลัง</v>
+      </c>
+      <c r="D21" t="str">
+        <v>เปลี่ยนขนาดตัวอักษร</v>
+      </c>
+      <c r="E21" t="str">
+        <v>ซ่อนองค์ประกอบ</v>
+      </c>
+      <c r="F21" t="str">
+        <v>A</v>
+      </c>
+    </row>
+    <row r="22">
+      <c r="A22" t="str">
+        <v>React คืออะไร?</v>
+      </c>
+      <c r="B22" t="str">
+        <v>JavaScript Library สำหรับสร้าง UI</v>
+      </c>
+      <c r="C22" t="str">
+        <v>ภาษาโปรแกรมมิ่ง</v>
+      </c>
+      <c r="D22" t="str">
+        <v>ฐานข้อมูล</v>
+      </c>
+      <c r="E22" t="str">
+        <v>Web Server</v>
+      </c>
+      <c r="F22" t="str">
+        <v>A</v>
+      </c>
+    </row>
+    <row r="23">
+      <c r="A23" t="str">
+        <v>Component ใน React คืออะไร?</v>
+      </c>
+      <c r="B23" t="str">
+        <v>Building block ของ UI</v>
+      </c>
+      <c r="C23" t="str">
+        <v>ฐานข้อมูล</v>
+      </c>
+      <c r="D23" t="str">
+        <v>API</v>
+      </c>
+      <c r="E23" t="str">
+        <v>CSS Framework</v>
+      </c>
+      <c r="F23" t="str">
+        <v>A</v>
+      </c>
+    </row>
+    <row r="24">
+      <c r="A24" t="str">
+        <v>useState Hook ใช้ทำอะไร?</v>
+      </c>
+      <c r="B24" t="str">
+        <v>จัดการ State</v>
+      </c>
+      <c r="C24" t="str">
+        <v>เรียก API</v>
+      </c>
+      <c r="D24" t="str">
+        <v>สร้าง Component</v>
+      </c>
+      <c r="E24" t="str">
+        <v>จัดการ Style</v>
+      </c>
+      <c r="F24" t="str">
+        <v>A</v>
+      </c>
+    </row>
+    <row r="25">
+      <c r="A25" t="str">
+        <v>useEffect Hook ใช้ทำอะไร?</v>
+      </c>
+      <c r="B25" t="str">
+        <v>จัดการ Side Effects</v>
+      </c>
+      <c r="C25" t="str">
+        <v>สร้างตัวแปร</v>
+      </c>
+      <c r="D25" t="str">
+        <v>ลบข้อมูล</v>
+      </c>
+      <c r="E25" t="str">
+        <v>ตรวจสอบ Error</v>
+      </c>
+      <c r="F25" t="str">
+        <v>A</v>
+      </c>
+    </row>
+    <row r="26">
+      <c r="A26" t="str">
+        <v>Props ใน React คืออะไร?</v>
+      </c>
+      <c r="B26" t="str">
+        <v>ข้อมูลที่ส่งระหว่าง Component</v>
+      </c>
+      <c r="C26" t="str">
+        <v>CSS Properties</v>
+      </c>
+      <c r="D26" t="str">
+        <v>JavaScript Properties</v>
+      </c>
+      <c r="E26" t="str">
+        <v>HTML Attributes</v>
+      </c>
+      <c r="F26" t="str">
+        <v>A</v>
+      </c>
+    </row>
+    <row r="27">
+      <c r="A27" t="str">
+        <v>Virtual DOM ใน React คืออะไร?</v>
+      </c>
+      <c r="B27" t="str">
+        <v>สำเนาของ Real DOM ในหน่วยความจำ</v>
+      </c>
+      <c r="C27" t="str">
+        <v>Database</v>
+      </c>
+      <c r="D27" t="str">
+        <v>API</v>
+      </c>
+      <c r="E27" t="str">
+        <v>Web Server</v>
+      </c>
+      <c r="F27" t="str">
+        <v>A</v>
+      </c>
+    </row>
+    <row r="28">
+      <c r="A28" t="str">
+        <v>JSX คืออะไร?</v>
+      </c>
+      <c r="B28" t="str">
+        <v>JavaScript XML</v>
+      </c>
+      <c r="C28" t="str">
+        <v>Java Syntax Extension</v>
+      </c>
+      <c r="D28" t="str">
+        <v>JSON XML</v>
+      </c>
+      <c r="E28" t="str">
+        <v>JavaScript Extension</v>
+      </c>
+      <c r="F28" t="str">
+        <v>A</v>
+      </c>
+    </row>
+    <row r="29">
+      <c r="A29" t="str">
+        <v>Key prop ใน React ใช้ทำไม?</v>
+      </c>
+      <c r="B29" t="str">
+        <v>ระบุ unique ID ใน list</v>
+      </c>
+      <c r="C29" t="str">
+        <v>เข้ารหัสข้อมูล</v>
+      </c>
+      <c r="D29" t="str">
+        <v>เปิดล็อค Component</v>
+      </c>
+      <c r="E29" t="str">
+        <v>จัดเรียงข้อมูล</v>
+      </c>
+      <c r="F29" t="str">
+        <v>A</v>
+      </c>
+    </row>
+    <row r="30">
+      <c r="A30" t="str">
+        <v>Context API ใช้ทำอะไร?</v>
+      </c>
+      <c r="B30" t="str">
+        <v>แชร์ข้อมูลข้าม Component</v>
+      </c>
+      <c r="C30" t="str">
+        <v>สร้าง API</v>
+      </c>
+      <c r="D30" t="str">
+        <v>จัดการ Database</v>
+      </c>
+      <c r="E30" t="str">
+        <v>เรียก HTTP Request</v>
+      </c>
+      <c r="F30" t="str">
+        <v>A</v>
+      </c>
+    </row>
+    <row r="31">
+      <c r="A31" t="str">
+        <v>React Router ใช้ทำอะไร?</v>
+      </c>
+      <c r="B31" t="str">
+        <v>จัดการ Navigation</v>
+      </c>
+      <c r="C31" t="str">
+        <v>จัดการ State</v>
+      </c>
+      <c r="D31" t="str">
+        <v>จัดการ Style</v>
+      </c>
+      <c r="E31" t="str">
+        <v>จัดการ Database</v>
+      </c>
+      <c r="F31" t="str">
+        <v>A</v>
       </c>
     </row>
   </sheetData>
   <ignoredErrors>
-    <ignoredError numberStoredAsText="1" sqref="A1:F4"/>
+    <ignoredError numberStoredAsText="1" sqref="A1:F31"/>
   </ignoredErrors>
 </worksheet>
 </file>
</xml_diff>